<commit_message>
update to realign with csv data
</commit_message>
<xml_diff>
--- a/template/xl-template.xlsx
+++ b/template/xl-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\Personal Stuff\Coding\Personal\Soundrop Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\Personal Stuff\Coding\Personal\Soundrop-Reports\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA29EC4D-0595-4A1C-8DB2-41100D17E89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BD76D0-22C2-447C-80BD-C95F8A18388C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -686,8 +686,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,9 +928,10 @@
       <c r="B43" s="7"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="11" t="s">
         <v>12</v>
       </c>
+      <c r="B44" s="13"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">

</xml_diff>